<commit_message>
Updating formulas when deleting a column
</commit_message>
<xml_diff>
--- a/_examples/spreadsheet/remove-column/original.xlsx
+++ b/_examples/spreadsheet/remove-column/original.xlsx
@@ -11,6 +11,13 @@
     <sheet name="Cells" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="MergedCells" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="false" name="cellsRange" vbProcedure="false">Cells!$A$3:$E$12</definedName>
+    <definedName function="false" hidden="false" name="check" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" name="columnsRange" vbProcedure="false">Cells!$B:$E</definedName>
+    <definedName function="false" hidden="false" name="rangeD" vbProcedure="false">Cells!$D$3:$D$12</definedName>
+    <definedName function="false" hidden="false" name="rangeE" vbProcedure="false">Cells!$E$3:$E$12</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -18,6 +25,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t xml:space="preserve">This should be kept after removing the column</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -116,10 +131,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:H12"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -127,6 +142,11 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K1" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1</v>
@@ -147,9 +167,13 @@
         <f aca="false">40+A3</f>
         <v>41</v>
       </c>
+      <c r="G3" s="0" t="n">
+        <f aca="false">50+E3</f>
+        <v>91</v>
+      </c>
       <c r="H3" s="0" t="n">
-        <f aca="false">50+A3</f>
-        <v>51</v>
+        <f aca="false">AVERAGE(D3:D12)*10</f>
+        <v>355</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -173,9 +197,13 @@
         <f aca="false">40+A4</f>
         <v>42</v>
       </c>
+      <c r="G4" s="0" t="n">
+        <f aca="false">50+E4</f>
+        <v>92</v>
+      </c>
       <c r="H4" s="0" t="n">
-        <f aca="false">50+A4</f>
-        <v>52</v>
+        <f aca="false">$E$4*100</f>
+        <v>4200</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -199,9 +227,13 @@
         <f aca="false">40+A5</f>
         <v>43</v>
       </c>
-      <c r="H5" s="0" t="n">
-        <f aca="false">50+A5</f>
-        <v>53</v>
+      <c r="G5" s="0" t="n">
+        <f aca="false">50+E5</f>
+        <v>93</v>
+      </c>
+      <c r="H5" s="0" t="str">
+        <f aca="false">IF(E5&lt;50,"E5","Hello world")</f>
+        <v>E5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -225,9 +257,9 @@
         <f aca="false">40+A6</f>
         <v>44</v>
       </c>
-      <c r="H6" s="0" t="n">
-        <f aca="false">50+A6</f>
-        <v>54</v>
+      <c r="G6" s="0" t="n">
+        <f aca="false">50+E6</f>
+        <v>94</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -251,9 +283,9 @@
         <f aca="false">40+A7</f>
         <v>45</v>
       </c>
-      <c r="H7" s="0" t="n">
-        <f aca="false">50+A7</f>
-        <v>55</v>
+      <c r="G7" s="0" t="n">
+        <f aca="false">50+E7</f>
+        <v>95</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -277,9 +309,9 @@
         <f aca="false">40+A8</f>
         <v>46</v>
       </c>
-      <c r="H8" s="0" t="n">
-        <f aca="false">50+A8</f>
-        <v>56</v>
+      <c r="G8" s="0" t="n">
+        <f aca="false">50+E8</f>
+        <v>96</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -303,9 +335,9 @@
         <f aca="false">40+A9</f>
         <v>47</v>
       </c>
-      <c r="H9" s="0" t="n">
-        <f aca="false">50+A9</f>
-        <v>57</v>
+      <c r="G9" s="0" t="n">
+        <f aca="false">50+E9</f>
+        <v>97</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -329,9 +361,9 @@
         <f aca="false">40+A10</f>
         <v>48</v>
       </c>
-      <c r="H10" s="0" t="n">
-        <f aca="false">50+A10</f>
-        <v>58</v>
+      <c r="G10" s="0" t="n">
+        <f aca="false">50+E10</f>
+        <v>98</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -355,9 +387,9 @@
         <f aca="false">40+A11</f>
         <v>49</v>
       </c>
-      <c r="H11" s="0" t="n">
-        <f aca="false">50+A11</f>
-        <v>59</v>
+      <c r="G11" s="0" t="n">
+        <f aca="false">50+E11</f>
+        <v>99</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -381,9 +413,27 @@
         <f aca="false">40+A12</f>
         <v>50</v>
       </c>
-      <c r="H12" s="0" t="n">
-        <f aca="false">50+A12</f>
-        <v>60</v>
+      <c r="G12" s="0" t="n">
+        <f aca="false">50+E12</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F14" s="0" t="n">
+        <f aca="false">SUM(cellsRange)</f>
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F15" s="0" t="n">
+        <f aca="false">MergedCells!G11+G12</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F16" s="0" t="n">
+        <f aca="false">F15</f>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -404,8 +454,8 @@
   </sheetPr>
   <dimension ref="B9:M32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -423,7 +473,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="H9" s="0" t="n">
+      <c r="G9" s="0" t="n">
         <v>11</v>
       </c>
     </row>
@@ -433,11 +483,57 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>6</v>
       </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
       <c r="H21" s="1" t="n">
         <v>9</v>
       </c>

</xml_diff>